<commit_message>
Finetuning the gpt prompt
</commit_message>
<xml_diff>
--- a/src/backend/resources/uploads/data.xlsx
+++ b/src/backend/resources/uploads/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trado7-my.sharepoint.com/personal/johannes_theisen_asklio_ai/Documents/RTSH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarac\Documents\GitHub\3NY\src\backend\resources\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{62614068-3087-5F41-81DB-2D9EC7ECD209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31C634D6-16C6-F448-88F8-7F00922554AB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5233AA34-AC67-4755-A446-3185A49AE548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1360" windowWidth="28240" windowHeight="17240" activeTab="2" xr2:uid="{54696791-7F2F-9443-8AAB-C526A8D12B52}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{54696791-7F2F-9443-8AAB-C526A8D12B52}"/>
   </bookViews>
   <sheets>
     <sheet name="vendors" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="154">
   <si>
     <t>name</t>
   </si>
@@ -347,9 +347,6 @@
   </si>
   <si>
     <t>Offers Travel tumblers, Insulated water bottles for promotional and giveaway purposes.</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>Name</t>
@@ -509,7 +506,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -872,18 +869,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291530D0-BB1C-0F42-A004-8B904714312E}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -897,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>4800</v>
       </c>
@@ -911,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>4801</v>
       </c>
@@ -925,7 +922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4802</v>
       </c>
@@ -939,7 +936,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4803</v>
       </c>
@@ -953,7 +950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4804</v>
       </c>
@@ -967,7 +964,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>4805</v>
       </c>
@@ -981,7 +978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>4806</v>
       </c>
@@ -995,7 +992,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>4807</v>
       </c>
@@ -1009,7 +1006,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>4808</v>
       </c>
@@ -1023,7 +1020,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>4809</v>
       </c>
@@ -1037,7 +1034,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>4810</v>
       </c>
@@ -1051,7 +1048,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>4811</v>
       </c>
@@ -1065,7 +1062,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>4812</v>
       </c>
@@ -1079,7 +1076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>4813</v>
       </c>
@@ -1093,7 +1090,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>4814</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4815</v>
       </c>
@@ -1121,7 +1118,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>4816</v>
       </c>
@@ -1135,7 +1132,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>4817</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>4818</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>4819</v>
       </c>
@@ -1177,7 +1174,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>4820</v>
       </c>
@@ -1191,7 +1188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>4821</v>
       </c>
@@ -1205,7 +1202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>4822</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>4823</v>
       </c>
@@ -1233,7 +1230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>4824</v>
       </c>
@@ -1247,7 +1244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>4825</v>
       </c>
@@ -1261,7 +1258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>4826</v>
       </c>
@@ -1275,7 +1272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>4827</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>4828</v>
       </c>
@@ -1303,7 +1300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>4829</v>
       </c>
@@ -1317,7 +1314,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>4830</v>
       </c>
@@ -1331,7 +1328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="18.95" customHeight="1">
       <c r="A33" s="1">
         <v>4831</v>
       </c>
@@ -1345,7 +1342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>4900</v>
       </c>
@@ -1359,7 +1356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>4901</v>
       </c>
@@ -1373,7 +1370,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>4902</v>
       </c>
@@ -1387,7 +1384,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>4903</v>
       </c>
@@ -1401,7 +1398,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>4904</v>
       </c>
@@ -1415,7 +1412,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>4905</v>
       </c>
@@ -1429,7 +1426,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>4906</v>
       </c>
@@ -1443,7 +1440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>4907</v>
       </c>
@@ -1457,7 +1454,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>4908</v>
       </c>
@@ -1471,7 +1468,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>4909</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>4910</v>
       </c>
@@ -1499,7 +1496,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>4911</v>
       </c>
@@ -1513,7 +1510,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>4912</v>
       </c>
@@ -1527,7 +1524,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>4913</v>
       </c>
@@ -1541,7 +1538,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>4914</v>
       </c>
@@ -1555,7 +1552,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>4915</v>
       </c>
@@ -1569,7 +1566,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>4916</v>
       </c>
@@ -1583,7 +1580,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>4917</v>
       </c>
@@ -1597,7 +1594,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>4918</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>4919</v>
       </c>
@@ -1634,248 +1631,249 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B69FD8-74C8-054B-9A9C-10818EE0D31A}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
-        <v>104</v>
-      </c>
       <c r="C1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
       <c r="C5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" t="s">
         <v>125</v>
-      </c>
-      <c r="C21" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1883,60 +1881,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0986165-1D7D-5045-BFF8-20732BEC812A}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G2" s="2">
         <v>120</v>
@@ -1971,7 +1969,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1988,7 +1986,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G3" s="2">
         <v>50</v>
@@ -2006,7 +2004,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2023,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G4" s="2">
         <v>15</v>
@@ -2041,7 +2039,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2058,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -2076,7 +2074,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2093,7 +2091,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6" s="2">
         <v>180</v>
@@ -2111,7 +2109,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -2128,7 +2126,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G7" s="2">
         <v>170</v>
@@ -2146,7 +2144,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G8" s="2">
         <v>25</v>
@@ -2181,7 +2179,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -2198,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G9" s="2">
         <v>110</v>
@@ -2216,7 +2214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -2233,7 +2231,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G10" s="2">
         <v>200</v>
@@ -2251,7 +2249,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -2268,7 +2266,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G11" s="2">
         <v>30</v>
@@ -2286,7 +2284,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -2303,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G12" s="2">
         <v>100</v>
@@ -2321,7 +2319,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -2338,7 +2336,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="2">
         <v>360</v>
@@ -2356,7 +2354,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2373,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G14" s="2">
         <v>30</v>
@@ -2391,7 +2389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -2408,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G15" s="2">
         <v>30</v>
@@ -2426,7 +2424,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -2443,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G16" s="2">
         <v>95</v>
@@ -2461,7 +2459,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -2478,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G17" s="2">
         <v>15</v>
@@ -2496,7 +2494,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -2513,7 +2511,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G18" s="2">
         <v>170</v>
@@ -2531,7 +2529,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -2548,7 +2546,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G19" s="2">
         <v>80</v>
@@ -2566,7 +2564,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="1">
         <v>10</v>
       </c>
@@ -2583,7 +2581,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G20" s="2">
         <v>100</v>
@@ -2601,7 +2599,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>11</v>
       </c>
@@ -2618,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G21" s="2">
         <v>40</v>
@@ -2636,7 +2634,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="1">
         <v>12</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G22" s="2">
         <v>360</v>
@@ -2662,7 +2660,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="1">
         <v>12</v>
       </c>
@@ -2679,7 +2677,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G23" s="2">
         <v>50</v>
@@ -2688,7 +2686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -2705,7 +2703,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G24" s="2">
         <v>80</v>
@@ -2714,7 +2712,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -2731,7 +2729,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G25" s="2">
         <v>20</v>
@@ -2740,7 +2738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" s="1">
         <v>13</v>
       </c>
@@ -2757,7 +2755,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G26" s="2">
         <v>150</v>
@@ -2766,7 +2764,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" s="1">
         <v>13</v>
       </c>
@@ -2783,7 +2781,7 @@
         <v>3</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G27" s="2">
         <v>120</v>
@@ -2792,7 +2790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" s="1">
         <v>14</v>
       </c>
@@ -2809,7 +2807,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G28" s="2">
         <v>20</v>
@@ -2818,7 +2816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" s="1">
         <v>14</v>
       </c>
@@ -2835,7 +2833,7 @@
         <v>3</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G29" s="2">
         <v>60</v>
@@ -2844,7 +2842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" s="1">
         <v>14</v>
       </c>
@@ -2861,7 +2859,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G30" s="2">
         <v>100</v>
@@ -2870,7 +2868,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="1">
         <v>15</v>
       </c>
@@ -2887,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G31" s="2">
         <v>220</v>
@@ -2896,7 +2894,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="1">
         <v>15</v>
       </c>
@@ -2913,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G32" s="2">
         <v>60</v>
@@ -2922,7 +2920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>16</v>
       </c>
@@ -2939,7 +2937,7 @@
         <v>3</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G33" s="2">
         <v>360</v>
@@ -2948,7 +2946,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>17</v>
       </c>
@@ -2965,7 +2963,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" s="2">
         <v>45</v>
@@ -2974,7 +2972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>18</v>
       </c>
@@ -2991,7 +2989,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G35" s="2">
         <v>20</v>
@@ -3000,7 +2998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>18</v>
       </c>
@@ -3017,7 +3015,7 @@
         <v>2</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G36" s="2">
         <v>170</v>
@@ -3026,7 +3024,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>18</v>
       </c>
@@ -3043,7 +3041,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G37" s="2">
         <v>95</v>
@@ -3052,7 +3050,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>19</v>
       </c>
@@ -3069,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G38" s="2">
         <v>10</v>
@@ -3078,7 +3076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>19</v>
       </c>
@@ -3095,7 +3093,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G39" s="2">
         <v>190</v>
@@ -3104,7 +3102,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>20</v>
       </c>
@@ -3121,7 +3119,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G40" s="2">
         <v>120</v>
@@ -3130,7 +3128,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>20</v>
       </c>
@@ -3147,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G41" s="2">
         <v>100</v>
@@ -3156,7 +3154,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>20</v>
       </c>
@@ -3173,7 +3171,7 @@
         <v>3</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G42" s="2">
         <v>285</v>

</xml_diff>